<commit_message>
Aula 06 - modelagem de dados
</commit_message>
<xml_diff>
--- a/Banco de dados/Modelagem Banco de Dados/Aula 05/excel/Aula 05 - Modelagem de dados.xlsx
+++ b/Banco de dados/Modelagem Banco de Dados/Aula 05/excel/Aula 05 - Modelagem de dados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisc\Documents\GitHub\aulas-graduacao\Banco de dados\Modelagem Banco de Dados\Aula 05\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ADEECCF5-C6ED-49F7-BAB9-D044757214A0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56750BA-9BA6-45C2-A5F8-58B21EE243ED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="4" activeTab="9" xr2:uid="{B4E6D965-D79E-4F5E-AD00-382A57D949CD}"/>
+    <workbookView xWindow="3690" yWindow="1800" windowWidth="28800" windowHeight="11505" xr2:uid="{B4E6D965-D79E-4F5E-AD00-382A57D949CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Entidades Fortes" sheetId="1" r:id="rId1"/>
@@ -1965,7 +1965,7 @@
   </sheetPr>
   <dimension ref="B2:K9"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
@@ -2060,7 +2060,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57D1C715-C757-41DB-8E92-BED6D62B4E7A}">
   <dimension ref="C2:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
@@ -2633,7 +2633,7 @@
   </sheetPr>
   <dimension ref="B3:K16"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>

</xml_diff>